<commit_message>
Clean up CE_b files as well as more value conversions to avoid problems. Also inlude all processed files for CE_b
</commit_message>
<xml_diff>
--- a/input/TRNSYS/14.02.RE/Std140_CE_b_Output.xlsx
+++ b/input/TRNSYS/14.02.RE/Std140_CE_b_Output.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\TRNSYS\14.02.RE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{820FFDE0-9093-4AD2-A299-CF279314EE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770B6C49-9D8F-4EE5-940F-8A9716B64D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7815" yWindow="1620" windowWidth="30675" windowHeight="17970" xr2:uid="{5500947F-28FA-4902-B983-E90B599A579F}"/>
+    <workbookView xWindow="10275" yWindow="1020" windowWidth="40575" windowHeight="15465" xr2:uid="{5500947F-28FA-4902-B983-E90B599A579F}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_Fill" hidden="1">#REF!</definedName>
   </definedNames>
@@ -455,12 +452,6 @@
     <t>E522</t>
   </si>
   <si>
-    <t>12-Mai</t>
-  </si>
-  <si>
-    <t>02-Mai</t>
-  </si>
-  <si>
     <t>E525</t>
   </si>
   <si>
@@ -470,9 +461,6 @@
     <t>E530</t>
   </si>
   <si>
-    <t>29-Mai</t>
-  </si>
-  <si>
     <t>18-Jun</t>
   </si>
   <si>
@@ -644,9 +632,6 @@
     <t>12</t>
   </si>
   <si>
-    <t>12-Dez</t>
-  </si>
-  <si>
     <t>28-Apr</t>
   </si>
   <si>
@@ -705,9 +690,6 @@
   </si>
   <si>
     <t>14-Jul</t>
-  </si>
-  <si>
-    <t>10-Mai</t>
   </si>
   <si>
     <t>12-Nov</t>
@@ -780,6 +762,21 @@
   </si>
   <si>
     <t xml:space="preserve">      C a s e   E 5 3 0   A v e r a g e   D a i l y   O u t p u t s  -  f(ODB) sensitivity</t>
+  </si>
+  <si>
+    <t>12-May</t>
+  </si>
+  <si>
+    <t>02-May</t>
+  </si>
+  <si>
+    <t>29-May</t>
+  </si>
+  <si>
+    <t>12-Dec</t>
+  </si>
+  <si>
+    <t>10-May</t>
   </si>
 </sst>
 </file>
@@ -1193,6 +1190,12 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1201,12 +1204,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1223,116 +1220,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Read Me"/>
-      <sheetName val="Adding Results"/>
-      <sheetName val="YourData"/>
-      <sheetName val="Title Page"/>
-      <sheetName val="Program List"/>
-      <sheetName val="Tables List"/>
-      <sheetName val="Figures List"/>
-      <sheetName val="Table-Q"/>
-      <sheetName val="Table-R"/>
-      <sheetName val="Table-S"/>
-      <sheetName val="Table-T"/>
-      <sheetName val="Fig B16.5.2-1 Qtot"/>
-      <sheetName val="Fig B16.5.2-2 dQtot"/>
-      <sheetName val="Fig B16.5.2-3 Ptot"/>
-      <sheetName val="Fig B16.5.2-4 dPtot"/>
-      <sheetName val="Fig B16.5.2-5 Qcomp"/>
-      <sheetName val="Fig B16.5.2-6 dQcomp"/>
-      <sheetName val="Fig B16.5.2-7 Qidfan"/>
-      <sheetName val="Fig B16.5.2-8 dQidfan"/>
-      <sheetName val="Fig B16.5.2-9 Qodfan"/>
-      <sheetName val="Fig B16.5.2-10 dQodfan"/>
-      <sheetName val="Fig B16.5.2-11 QCtot"/>
-      <sheetName val="Fig B16.5.2-12 PCtot"/>
-      <sheetName val="Fig B16.5.2-13 dPCtot"/>
-      <sheetName val="Fig B16.5.2-14 QCSens"/>
-      <sheetName val="Fig B16.5.2-15 dQCsens"/>
-      <sheetName val="Fig B16.5.2-16 PCSens"/>
-      <sheetName val="Fig B16.5.2-17 QClat"/>
-      <sheetName val="Fig B16.5.2-18 dQClat"/>
-      <sheetName val="Fig B16.5.2-19 PClat"/>
-      <sheetName val="Fig B16.5.2-20 dPClat"/>
-      <sheetName val="Fig B16.5.2-21 COP2"/>
-      <sheetName val="Fig B16.5.2-22 dCOP2"/>
-      <sheetName val="Fig B16.5.2-23 MxCOP2"/>
-      <sheetName val="Fig B16.5.2-24 dMxCOP2"/>
-      <sheetName val="Fig B16.5.2-25 MnCOP2"/>
-      <sheetName val="Fig B16.5.2-26 dMnCOP2"/>
-      <sheetName val="Fig B16.5.2-27 IDB"/>
-      <sheetName val="Fig B16.5.2-28 dIDB"/>
-      <sheetName val="Fig B16.5.2-29 MxIDB"/>
-      <sheetName val="Fig B16.5.2-30 dMxIDB"/>
-      <sheetName val="Fig B16.5.2-31 MnIDB"/>
-      <sheetName val="Fig B16.5.2-32 Humrat"/>
-      <sheetName val="Fig B16.5.2-33 dHumrat"/>
-      <sheetName val="Fig B16.5.2-34 MxHum"/>
-      <sheetName val="Fig B16.5.2-35 dMxHumrat"/>
-      <sheetName val="Fig B16.5.2-36 MnHum"/>
-      <sheetName val="Fig B16.5.2-37 RelHum"/>
-      <sheetName val="Fig B16.5.2-38 dRelHum"/>
-      <sheetName val="Fig B16.5.2-39 MxRelHum"/>
-      <sheetName val="Fig B16.5.2-40 dMxRelHum"/>
-      <sheetName val="Fig B16.5.2-41 MnRelHum"/>
-      <sheetName val="Fig B16.5.2-42 Qf(ODB)"/>
-      <sheetName val="Fig B16.5.2-43 QCf(ODB)"/>
-      <sheetName val="Fig B16.5.2-44 COP2f(ODB)"/>
-      <sheetName val="Fig B16.5.2-45 Humratf(ODB)"/>
-      <sheetName val="Fig B16.5.2-46 HrQ"/>
-      <sheetName val="Fig B16.5.2-47 HrQC"/>
-      <sheetName val="Fig B16.5.2-48 HrCOP2"/>
-      <sheetName val="Fig B16.5.2-49 HrHum"/>
-      <sheetName val="Fig B16.5.2-50 HrEDB,EWB"/>
-      <sheetName val="Fig B16.5.2-51 HrODB"/>
-      <sheetName val="Fig B16.5.2-52 HrOHR"/>
-      <sheetName val="A"/>
-      <sheetName val="Qdata"/>
-      <sheetName val="Rdata"/>
-      <sheetName val="Sdata"/>
-      <sheetName val="Tdata"/>
-      <sheetName val="TRNSYS-TUD"/>
-      <sheetName val="DOE22"/>
-      <sheetName val="DOE21E"/>
-      <sheetName val="EnergyPlus1.0"/>
-      <sheetName val="CodyRun"/>
-      <sheetName val="HOT3000"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-      <sheetData sheetId="66"/>
-      <sheetData sheetId="67"/>
-      <sheetData sheetId="68"/>
-      <sheetData sheetId="69"/>
-      <sheetData sheetId="70"/>
-      <sheetData sheetId="71"/>
-      <sheetData sheetId="72"/>
-      <sheetData sheetId="73"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1657,8 +1544,8 @@
   </sheetPr>
   <dimension ref="A1:AN130"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A42" colorId="22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A39" colorId="22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X106" sqref="X106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.6640625" defaultRowHeight="15"/>
@@ -3596,8 +3483,8 @@
       <c r="T77" s="22">
         <v>19488.8</v>
       </c>
-      <c r="U77" s="26" t="s">
-        <v>137</v>
+      <c r="U77" s="56" t="s">
+        <v>238</v>
       </c>
       <c r="V77" s="26">
         <v>15</v>
@@ -3605,8 +3492,8 @@
       <c r="W77" s="22">
         <v>7906.7</v>
       </c>
-      <c r="X77" s="26" t="s">
-        <v>138</v>
+      <c r="X77" s="56" t="s">
+        <v>239</v>
       </c>
       <c r="Y77" s="26">
         <v>15</v>
@@ -3614,8 +3501,8 @@
       <c r="Z77" s="22">
         <v>27383.59</v>
       </c>
-      <c r="AA77" s="26" t="s">
-        <v>137</v>
+      <c r="AA77" s="56" t="s">
+        <v>238</v>
       </c>
       <c r="AB77" s="29">
         <v>15</v>
@@ -3665,7 +3552,7 @@
       <c r="N78" s="26"/>
       <c r="O78" s="26"/>
       <c r="P78" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="Q78" s="22">
         <v>9366.7480928703299</v>
@@ -3680,7 +3567,7 @@
         <v>19702.7</v>
       </c>
       <c r="U78" s="26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="V78" s="26">
         <v>16</v>
@@ -3689,7 +3576,7 @@
         <v>8037.07</v>
       </c>
       <c r="X78" s="26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Y78" s="26">
         <v>16</v>
@@ -3698,7 +3585,7 @@
         <v>27739.77</v>
       </c>
       <c r="AA78" s="26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AB78" s="29">
         <v>16</v>
@@ -3706,7 +3593,7 @@
     </row>
     <row r="79" spans="1:28" ht="15.75">
       <c r="A79" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B79" s="22">
         <f t="shared" si="0"/>
@@ -3748,7 +3635,7 @@
       <c r="N79" s="26"/>
       <c r="O79" s="26"/>
       <c r="P79" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Q79" s="22">
         <v>8028.3285466124171</v>
@@ -3762,8 +3649,8 @@
       <c r="T79" s="22">
         <v>19834.099999999999</v>
       </c>
-      <c r="U79" s="26" t="s">
-        <v>142</v>
+      <c r="U79" s="56" t="s">
+        <v>240</v>
       </c>
       <c r="V79" s="26">
         <v>15</v>
@@ -3772,7 +3659,7 @@
         <v>1.6431299999999999E-11</v>
       </c>
       <c r="X79" s="26" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="Y79" s="26">
         <v>16</v>
@@ -3780,8 +3667,8 @@
       <c r="Z79" s="22">
         <v>19834.099999999999</v>
       </c>
-      <c r="AA79" s="26" t="s">
-        <v>142</v>
+      <c r="AA79" s="56" t="s">
+        <v>240</v>
       </c>
       <c r="AB79" s="29">
         <v>15</v>
@@ -3789,7 +3676,7 @@
     </row>
     <row r="80" spans="1:28" ht="15.75">
       <c r="A80" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B80" s="22">
         <f t="shared" si="0"/>
@@ -3831,7 +3718,7 @@
       <c r="N80" s="26"/>
       <c r="O80" s="26"/>
       <c r="P80" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q80" s="22">
         <v>8698.956160670863</v>
@@ -3846,7 +3733,7 @@
         <v>19575</v>
       </c>
       <c r="U80" s="26" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="V80" s="26">
         <v>16</v>
@@ -3855,7 +3742,7 @@
         <v>627.18600000000004</v>
       </c>
       <c r="X80" s="26" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="Y80" s="26">
         <v>10</v>
@@ -3864,7 +3751,7 @@
         <v>19575</v>
       </c>
       <c r="AA80" s="26" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AB80" s="29">
         <v>16</v>
@@ -3872,7 +3759,7 @@
     </row>
     <row r="81" spans="1:40" ht="15.75">
       <c r="A81" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B81" s="22">
         <f t="shared" si="0"/>
@@ -3914,7 +3801,7 @@
       <c r="N81" s="26"/>
       <c r="O81" s="26"/>
       <c r="P81" s="12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q81" s="40">
         <v>7204.8270241150658</v>
@@ -3929,7 +3816,7 @@
         <v>20075.2</v>
       </c>
       <c r="U81" s="41" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="V81" s="41">
         <v>16</v>
@@ -3938,7 +3825,7 @@
         <v>1.81188E-11</v>
       </c>
       <c r="X81" s="41" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="Y81" s="41">
         <v>16</v>
@@ -3947,7 +3834,7 @@
         <v>20075.2</v>
       </c>
       <c r="AA81" s="41" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AB81" s="42">
         <v>16</v>
@@ -3955,7 +3842,7 @@
     </row>
     <row r="82" spans="1:40" ht="15.75">
       <c r="A82" s="12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B82" s="40">
         <f>C82+D82+E82</f>
@@ -4003,7 +3890,7 @@
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
@@ -4017,7 +3904,7 @@
       <c r="R84" s="7"/>
       <c r="S84" s="7"/>
       <c r="T84" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="U84" s="7"/>
       <c r="V84" s="7"/>
@@ -4082,10 +3969,10 @@
     <row r="86" spans="1:40">
       <c r="A86" s="11"/>
       <c r="B86" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G86" s="18" t="s">
         <v>71</v>
@@ -4093,24 +3980,24 @@
       <c r="H86" s="45"/>
       <c r="K86" s="8"/>
       <c r="L86" s="46" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="P86" s="11"/>
       <c r="Q86" s="11"/>
       <c r="S86" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W86" s="11"/>
       <c r="X86" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="AC86" s="11"/>
       <c r="AD86" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AI86" s="11"/>
       <c r="AJ86" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="AN86" s="16"/>
     </row>
@@ -4134,79 +4021,79 @@
         <v>86</v>
       </c>
       <c r="G87" s="18" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H87" s="47" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I87" s="2" t="s">
         <v>90</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K87" s="15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="L87" s="15" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="P87" s="11" t="s">
         <v>80</v>
       </c>
       <c r="Q87" s="11"/>
       <c r="R87" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="T87" s="11"/>
       <c r="U87" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="W87" s="11"/>
       <c r="X87" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="Z87" s="11"/>
       <c r="AA87" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AC87" s="11"/>
       <c r="AD87" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="AF87" s="11"/>
       <c r="AG87" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AI87" s="11"/>
       <c r="AJ87" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AL87" s="11"/>
       <c r="AM87" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AN87" s="16"/>
     </row>
     <row r="88" spans="1:40">
       <c r="A88" s="12"/>
       <c r="B88" s="19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D88" s="19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E88" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F88" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G88" s="19" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H88" s="48"/>
       <c r="I88" s="20" t="s">
@@ -4277,7 +4164,7 @@
         <v>60</v>
       </c>
       <c r="AI88" s="19" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AJ88" s="20" t="s">
         <v>59</v>
@@ -4286,7 +4173,7 @@
         <v>60</v>
       </c>
       <c r="AL88" s="19" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AM88" s="20" t="s">
         <v>59</v>
@@ -4297,7 +4184,7 @@
     </row>
     <row r="89" spans="1:40" ht="15.75">
       <c r="A89" s="11" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B89" s="22">
         <v>2055.769720310841</v>
@@ -4340,7 +4227,7 @@
         <v>4.1683375374401095</v>
       </c>
       <c r="R89" s="26" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="S89" s="26">
         <v>3</v>
@@ -4358,7 +4245,7 @@
         <v>26.1999</v>
       </c>
       <c r="X89" s="26" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="Y89" s="26">
         <v>15</v>
@@ -4367,7 +4254,7 @@
         <v>7.9299799999999996</v>
       </c>
       <c r="AA89" s="26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AB89" s="26">
         <v>6</v>
@@ -4376,7 +4263,7 @@
         <v>1.3284300000000001E-2</v>
       </c>
       <c r="AD89" s="26" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AE89" s="26">
         <v>17</v>
@@ -4385,7 +4272,7 @@
         <v>1.87685E-3</v>
       </c>
       <c r="AG89" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AH89" s="26">
         <v>3</v>
@@ -4394,7 +4281,7 @@
         <v>68.789199999999994</v>
       </c>
       <c r="AJ89" s="26" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AK89" s="26">
         <v>17</v>
@@ -4403,7 +4290,7 @@
         <v>13.331200000000001</v>
       </c>
       <c r="AM89" s="26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AN89" s="29">
         <v>5</v>
@@ -4411,7 +4298,7 @@
     </row>
     <row r="90" spans="1:40" ht="15.75">
       <c r="A90" s="11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B90" s="22">
         <v>2053.6705655900555</v>
@@ -4454,7 +4341,7 @@
         <v>4.1433004323979068</v>
       </c>
       <c r="R90" s="26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="S90" s="26">
         <v>15</v>
@@ -4463,7 +4350,7 @@
         <v>2.8652350328328815</v>
       </c>
       <c r="U90" s="26" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="V90" s="26">
         <v>15</v>
@@ -4481,7 +4368,7 @@
         <v>7.9299799999999996</v>
       </c>
       <c r="AA90" s="26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AB90" s="26">
         <v>6</v>
@@ -4499,7 +4386,7 @@
         <v>1.8768599999999999E-3</v>
       </c>
       <c r="AG90" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AH90" s="26">
         <v>3</v>
@@ -4517,7 +4404,7 @@
         <v>13.389799999999999</v>
       </c>
       <c r="AM90" s="26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AN90" s="29">
         <v>6</v>
@@ -4525,7 +4412,7 @@
     </row>
     <row r="91" spans="1:40" ht="15.75">
       <c r="A91" s="11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B91" s="22">
         <v>2054.4922521461531</v>
@@ -4568,7 +4455,7 @@
         <v>4.1683375374401095</v>
       </c>
       <c r="R91" s="26" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="S91" s="26">
         <v>3</v>
@@ -4577,7 +4464,7 @@
         <v>2.8252032267490548</v>
       </c>
       <c r="U91" s="26" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="V91" s="26">
         <v>14</v>
@@ -4595,7 +4482,7 @@
         <v>7.9299799999999996</v>
       </c>
       <c r="AA91" s="26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AB91" s="26">
         <v>6</v>
@@ -4604,7 +4491,7 @@
         <v>1.8016899999999999E-2</v>
       </c>
       <c r="AD91" s="26" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AE91" s="26">
         <v>13</v>
@@ -4613,7 +4500,7 @@
         <v>1.87685E-3</v>
       </c>
       <c r="AG91" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AH91" s="26">
         <v>3</v>
@@ -4631,7 +4518,7 @@
         <v>13.331200000000001</v>
       </c>
       <c r="AM91" s="26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AN91" s="29">
         <v>5</v>
@@ -4639,7 +4526,7 @@
     </row>
     <row r="92" spans="1:40" ht="15.75">
       <c r="A92" s="11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B92" s="22">
         <v>1830.0823980528924</v>
@@ -4682,7 +4569,7 @@
         <v>4.1683375374401095</v>
       </c>
       <c r="R92" s="26" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="S92" s="26">
         <v>3</v>
@@ -4691,7 +4578,7 @@
         <v>2.8252032267490548</v>
       </c>
       <c r="U92" s="26" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="V92" s="26">
         <v>14</v>
@@ -4709,7 +4596,7 @@
         <v>7.9299799999999996</v>
       </c>
       <c r="AA92" s="26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AB92" s="26">
         <v>6</v>
@@ -4718,7 +4605,7 @@
         <v>1.7651400000000001E-2</v>
       </c>
       <c r="AD92" s="26" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AE92" s="26">
         <v>12</v>
@@ -4727,7 +4614,7 @@
         <v>1.87685E-3</v>
       </c>
       <c r="AG92" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AH92" s="26">
         <v>3</v>
@@ -4736,7 +4623,7 @@
         <v>76.659099999999995</v>
       </c>
       <c r="AJ92" s="26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="AK92" s="26">
         <v>20</v>
@@ -4745,7 +4632,7 @@
         <v>13.331200000000001</v>
       </c>
       <c r="AM92" s="26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AN92" s="29">
         <v>5</v>
@@ -4753,7 +4640,7 @@
     </row>
     <row r="93" spans="1:40" ht="15.75">
       <c r="A93" s="11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B93" s="22">
         <v>2029.3425670209424</v>
@@ -4796,7 +4683,7 @@
         <v>4.1683375374401095</v>
       </c>
       <c r="R93" s="26" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="S93" s="26">
         <v>3</v>
@@ -4805,7 +4692,7 @@
         <v>2.8252032267490548</v>
       </c>
       <c r="U93" s="26" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="V93" s="26">
         <v>14</v>
@@ -4823,7 +4710,7 @@
         <v>7.9299799999999996</v>
       </c>
       <c r="AA93" s="26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AB93" s="26">
         <v>6</v>
@@ -4832,7 +4719,7 @@
         <v>1.7871399999999999E-2</v>
       </c>
       <c r="AD93" s="26" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AE93" s="26">
         <v>13</v>
@@ -4841,7 +4728,7 @@
         <v>1.87685E-3</v>
       </c>
       <c r="AG93" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AH93" s="26">
         <v>3</v>
@@ -4859,7 +4746,7 @@
         <v>13.331200000000001</v>
       </c>
       <c r="AM93" s="26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AN93" s="29">
         <v>5</v>
@@ -4867,7 +4754,7 @@
     </row>
     <row r="94" spans="1:40" ht="15.75">
       <c r="A94" s="11" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B94" s="22">
         <v>1839.4316687849705</v>
@@ -4910,7 +4797,7 @@
         <v>4.1683375374401095</v>
       </c>
       <c r="R94" s="26" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="S94" s="26">
         <v>3</v>
@@ -4937,7 +4824,7 @@
         <v>7.9299799999999996</v>
       </c>
       <c r="AA94" s="26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AB94" s="26">
         <v>6</v>
@@ -4955,7 +4842,7 @@
         <v>1.87685E-3</v>
       </c>
       <c r="AG94" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AH94" s="26">
         <v>3</v>
@@ -4964,7 +4851,7 @@
         <v>68.789199999999994</v>
       </c>
       <c r="AJ94" s="26" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AK94" s="26">
         <v>17</v>
@@ -4973,7 +4860,7 @@
         <v>13.331200000000001</v>
       </c>
       <c r="AM94" s="26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AN94" s="29">
         <v>5</v>
@@ -4981,7 +4868,7 @@
     </row>
     <row r="95" spans="1:40" ht="15.75">
       <c r="A95" s="11" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B95" s="22">
         <v>2667.2443936627674</v>
@@ -5024,7 +4911,7 @@
         <v>4.4009649556697976</v>
       </c>
       <c r="R95" s="26" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="S95" s="26">
         <v>1</v>
@@ -5033,7 +4920,7 @@
         <v>2.8252032267490548</v>
       </c>
       <c r="U95" s="26" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="V95" s="26">
         <v>14</v>
@@ -5042,7 +4929,7 @@
         <v>33.758499999999998</v>
       </c>
       <c r="X95" s="26" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="Y95" s="26">
         <v>13</v>
@@ -5051,7 +4938,7 @@
         <v>7.9299799999999996</v>
       </c>
       <c r="AA95" s="26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AB95" s="26">
         <v>6</v>
@@ -5060,7 +4947,7 @@
         <v>1.34334E-2</v>
       </c>
       <c r="AD95" s="26" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AE95" s="26">
         <v>13</v>
@@ -5069,7 +4956,7 @@
         <v>1.87685E-3</v>
       </c>
       <c r="AG95" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AH95" s="26">
         <v>3</v>
@@ -5078,7 +4965,7 @@
         <v>68.789199999999994</v>
       </c>
       <c r="AJ95" s="26" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AK95" s="26">
         <v>17</v>
@@ -5087,7 +4974,7 @@
         <v>13.331200000000001</v>
       </c>
       <c r="AM95" s="26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AN95" s="29">
         <v>5</v>
@@ -5095,7 +4982,7 @@
     </row>
     <row r="96" spans="1:40" ht="15.75">
       <c r="A96" s="11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B96" s="22">
         <v>3552.7184949106027</v>
@@ -5147,7 +5034,7 @@
         <v>2.7819111679738864</v>
       </c>
       <c r="U96" s="26" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="V96" s="26">
         <v>19</v>
@@ -5165,7 +5052,7 @@
         <v>7.9299799999999996</v>
       </c>
       <c r="AA96" s="26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AB96" s="26">
         <v>6</v>
@@ -5174,7 +5061,7 @@
         <v>1.69436E-2</v>
       </c>
       <c r="AD96" s="26" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="AE96" s="26">
         <v>22</v>
@@ -5183,7 +5070,7 @@
         <v>1.87685E-3</v>
       </c>
       <c r="AG96" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AH96" s="26">
         <v>3</v>
@@ -5192,7 +5079,7 @@
         <v>83.753399999999999</v>
       </c>
       <c r="AJ96" s="26" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="AK96" s="26">
         <v>22</v>
@@ -5201,7 +5088,7 @@
         <v>13.209</v>
       </c>
       <c r="AM96" s="26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AN96" s="29">
         <v>5</v>
@@ -5209,7 +5096,7 @@
     </row>
     <row r="97" spans="1:40" ht="15.75">
       <c r="A97" s="11" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B97" s="22">
         <v>4364.7758495164062</v>
@@ -5252,7 +5139,7 @@
         <v>3.8879096164892295</v>
       </c>
       <c r="R97" s="26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="S97" s="26">
         <v>15</v>
@@ -5270,7 +5157,7 @@
         <v>26.825600000000001</v>
       </c>
       <c r="X97" s="26" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="Y97" s="26">
         <v>15</v>
@@ -5279,7 +5166,7 @@
         <v>7.9299799999999996</v>
       </c>
       <c r="AA97" s="26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AB97" s="26">
         <v>6</v>
@@ -5288,7 +5175,7 @@
         <v>1.68355E-2</v>
       </c>
       <c r="AD97" s="26" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="AE97" s="26">
         <v>22</v>
@@ -5297,7 +5184,7 @@
         <v>1.87685E-3</v>
       </c>
       <c r="AG97" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AH97" s="26">
         <v>3</v>
@@ -5306,7 +5193,7 @@
         <v>83.224699999999999</v>
       </c>
       <c r="AJ97" s="26" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="AK97" s="26">
         <v>22</v>
@@ -5315,7 +5202,7 @@
         <v>13.209099999999999</v>
       </c>
       <c r="AM97" s="26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AN97" s="29">
         <v>5</v>
@@ -5323,7 +5210,7 @@
     </row>
     <row r="98" spans="1:40" ht="15.75">
       <c r="A98" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B98" s="22">
         <v>4441.0632976815668</v>
@@ -5366,7 +5253,7 @@
         <v>3.7812884390914867</v>
       </c>
       <c r="R98" s="26" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="S98" s="26">
         <v>16</v>
@@ -5384,7 +5271,7 @@
         <v>26.1999</v>
       </c>
       <c r="X98" s="26" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="Y98" s="26">
         <v>15</v>
@@ -5393,7 +5280,7 @@
         <v>7.9299799999999996</v>
       </c>
       <c r="AA98" s="26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AB98" s="26">
         <v>6</v>
@@ -5402,7 +5289,7 @@
         <v>1.42968E-2</v>
       </c>
       <c r="AD98" s="26" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="AE98" s="26">
         <v>10</v>
@@ -5411,7 +5298,7 @@
         <v>1.87685E-3</v>
       </c>
       <c r="AG98" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AH98" s="26">
         <v>3</v>
@@ -5420,7 +5307,7 @@
         <v>70.841099999999997</v>
       </c>
       <c r="AJ98" s="26" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="AK98" s="26">
         <v>10</v>
@@ -5429,7 +5316,7 @@
         <v>13.209899999999999</v>
       </c>
       <c r="AM98" s="26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AN98" s="29">
         <v>5</v>
@@ -5437,7 +5324,7 @@
     </row>
     <row r="99" spans="1:40" ht="15.75">
       <c r="A99" s="11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B99" s="22">
         <v>4999.5949681009843</v>
@@ -5480,7 +5367,7 @@
         <v>3.7812884390914867</v>
       </c>
       <c r="R99" s="26" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="S99" s="26">
         <v>16</v>
@@ -5489,7 +5376,7 @@
         <v>2.7711375787107482</v>
       </c>
       <c r="U99" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="V99" s="26">
         <v>19</v>
@@ -5498,7 +5385,7 @@
         <v>27.199200000000001</v>
       </c>
       <c r="X99" s="26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="Y99" s="26">
         <v>16</v>
@@ -5507,7 +5394,7 @@
         <v>7.9299799999999996</v>
       </c>
       <c r="AA99" s="26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AB99" s="26">
         <v>6</v>
@@ -5516,7 +5403,7 @@
         <v>1.6230600000000001E-2</v>
       </c>
       <c r="AD99" s="26" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="AE99" s="26">
         <v>5</v>
@@ -5525,7 +5412,7 @@
         <v>1.87685E-3</v>
       </c>
       <c r="AG99" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AH99" s="26">
         <v>3</v>
@@ -5534,7 +5421,7 @@
         <v>80.708699999999993</v>
       </c>
       <c r="AJ99" s="26" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="AK99" s="26">
         <v>5</v>
@@ -5543,7 +5430,7 @@
         <v>13.207800000000001</v>
       </c>
       <c r="AM99" s="26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AN99" s="29">
         <v>5</v>
@@ -5551,7 +5438,7 @@
     </row>
     <row r="100" spans="1:40" ht="15.75">
       <c r="A100" s="11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B100" s="22">
         <v>5316.7711371459918</v>
@@ -5593,8 +5480,8 @@
       <c r="Q100" s="24">
         <v>3.8834748713994482</v>
       </c>
-      <c r="R100" s="26" t="s">
-        <v>200</v>
+      <c r="R100" s="56" t="s">
+        <v>241</v>
       </c>
       <c r="S100" s="26">
         <v>7</v>
@@ -5603,7 +5490,7 @@
         <v>2.7824815154757125</v>
       </c>
       <c r="U100" s="26" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="V100" s="26">
         <v>19</v>
@@ -5612,7 +5499,7 @@
         <v>27.045200000000001</v>
       </c>
       <c r="X100" s="26" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="Y100" s="26">
         <v>15</v>
@@ -5621,7 +5508,7 @@
         <v>7.9299799999999996</v>
       </c>
       <c r="AA100" s="26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AB100" s="26">
         <v>6</v>
@@ -5630,7 +5517,7 @@
         <v>1.33128E-2</v>
       </c>
       <c r="AD100" s="26" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AE100" s="26">
         <v>17</v>
@@ -5639,7 +5526,7 @@
         <v>1.87685E-3</v>
       </c>
       <c r="AG100" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AH100" s="26">
         <v>3</v>
@@ -5648,7 +5535,7 @@
         <v>68.724199999999996</v>
       </c>
       <c r="AJ100" s="26" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AK100" s="26">
         <v>17</v>
@@ -5657,7 +5544,7 @@
         <v>13.206899999999999</v>
       </c>
       <c r="AM100" s="56" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AN100" s="29">
         <v>5</v>
@@ -5665,7 +5552,7 @@
     </row>
     <row r="101" spans="1:40" ht="15.75">
       <c r="A101" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B101" s="22">
         <v>6188.547691714125</v>
@@ -5708,7 +5595,7 @@
         <v>4.2751401713091282</v>
       </c>
       <c r="R101" s="26" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="S101" s="26">
         <v>1</v>
@@ -5717,7 +5604,7 @@
         <v>2.6851972253498229</v>
       </c>
       <c r="U101" s="26" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="V101" s="26">
         <v>12</v>
@@ -5726,7 +5613,7 @@
         <v>25.805399999999999</v>
       </c>
       <c r="X101" s="26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Y101" s="26">
         <v>15</v>
@@ -5735,7 +5622,7 @@
         <v>8.4270099999999992</v>
       </c>
       <c r="AA101" s="26" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AB101" s="26">
         <v>22</v>
@@ -5744,7 +5631,7 @@
         <v>1.17197E-2</v>
       </c>
       <c r="AD101" s="26" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="AE101" s="26">
         <v>15</v>
@@ -5753,7 +5640,7 @@
         <v>6.8275599999999999E-3</v>
       </c>
       <c r="AG101" s="26" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AH101" s="26">
         <v>22</v>
@@ -5762,7 +5649,7 @@
         <v>100</v>
       </c>
       <c r="AJ101" s="56" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="AK101" s="26">
         <v>24</v>
@@ -5771,7 +5658,7 @@
         <v>53.4054</v>
       </c>
       <c r="AM101" s="56" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AN101" s="29">
         <v>15</v>
@@ -5779,7 +5666,7 @@
     </row>
     <row r="102" spans="1:40" ht="15.75">
       <c r="A102" s="11" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B102" s="22">
         <v>6210.9292642389719</v>
@@ -5822,7 +5709,7 @@
         <v>4.6925417995477332</v>
       </c>
       <c r="R102" s="26" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="S102" s="26">
         <v>1</v>
@@ -5831,7 +5718,7 @@
         <v>2.8879586954371632</v>
       </c>
       <c r="U102" s="26" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="V102" s="26">
         <v>15</v>
@@ -5840,7 +5727,7 @@
         <v>26.100300000000001</v>
       </c>
       <c r="X102" s="26" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="Y102" s="26">
         <v>15</v>
@@ -5849,7 +5736,7 @@
         <v>8.4270099999999992</v>
       </c>
       <c r="AA102" s="26" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AB102" s="26">
         <v>22</v>
@@ -5858,7 +5745,7 @@
         <v>1.1871400000000001E-2</v>
       </c>
       <c r="AD102" s="26" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="AE102" s="26">
         <v>15</v>
@@ -5867,7 +5754,7 @@
         <v>6.8275599999999999E-3</v>
       </c>
       <c r="AG102" s="26" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AH102" s="26">
         <v>22</v>
@@ -5876,7 +5763,7 @@
         <v>100</v>
       </c>
       <c r="AJ102" s="56" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="AK102" s="26">
         <v>24</v>
@@ -5885,7 +5772,7 @@
         <v>52.087899999999998</v>
       </c>
       <c r="AM102" s="56" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="AN102" s="29">
         <v>23</v>
@@ -5936,7 +5823,7 @@
         <v>3.8137362627521112</v>
       </c>
       <c r="R103" s="26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="S103" s="26">
         <v>15</v>
@@ -5945,7 +5832,7 @@
         <v>2.4416935229096444</v>
       </c>
       <c r="U103" s="26" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="V103" s="26">
         <v>12</v>
@@ -5954,7 +5841,7 @@
         <v>16.123200000000001</v>
       </c>
       <c r="X103" s="26" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="Y103" s="26">
         <v>15</v>
@@ -5963,7 +5850,7 @@
         <v>8.3052600000000005</v>
       </c>
       <c r="AA103" s="26" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AB103" s="26">
         <v>22</v>
@@ -5972,7 +5859,7 @@
         <v>7.5403099999999997E-3</v>
       </c>
       <c r="AD103" s="26" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="AE103" s="26">
         <v>15</v>
@@ -5981,7 +5868,7 @@
         <v>6.1029600000000002E-3</v>
       </c>
       <c r="AG103" s="56" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="AH103" s="26">
         <v>2</v>
@@ -5990,7 +5877,7 @@
         <v>90.229900000000001</v>
       </c>
       <c r="AJ103" s="56" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AK103" s="26">
         <v>22</v>
@@ -5999,7 +5886,7 @@
         <v>61.267899999999997</v>
       </c>
       <c r="AM103" s="56" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="AN103" s="29">
         <v>24</v>
@@ -6007,7 +5894,7 @@
     </row>
     <row r="104" spans="1:40" ht="15.75">
       <c r="A104" s="11" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B104" s="22">
         <v>7964.8229620022494</v>
@@ -6050,7 +5937,7 @@
         <v>3.9855085757608739</v>
       </c>
       <c r="R104" s="26" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="S104" s="26">
         <v>10</v>
@@ -6068,7 +5955,7 @@
         <v>21.0091</v>
       </c>
       <c r="X104" s="26" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="Y104" s="26">
         <v>15</v>
@@ -6077,7 +5964,7 @@
         <v>8.4140999999999995</v>
       </c>
       <c r="AA104" s="26" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AB104" s="26">
         <v>22</v>
@@ -6095,7 +5982,7 @@
         <v>6.8214900000000004E-3</v>
       </c>
       <c r="AG104" s="26" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AH104" s="26">
         <v>22</v>
@@ -6104,7 +5991,7 @@
         <v>100</v>
       </c>
       <c r="AJ104" s="56" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="AK104" s="26">
         <v>8</v>
@@ -6113,7 +6000,7 @@
         <v>58.505400000000002</v>
       </c>
       <c r="AM104" s="56" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AN104" s="29">
         <v>15</v>
@@ -6121,7 +6008,7 @@
     </row>
     <row r="105" spans="1:40" ht="15.75">
       <c r="A105" s="11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B105" s="22">
         <v>5420.7774972433799</v>
@@ -6158,13 +6045,13 @@
         <v>1.45051E-2</v>
       </c>
       <c r="P105" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="Q105" s="57">
         <v>4.7177562254396657</v>
       </c>
       <c r="R105" s="26" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="S105" s="26">
         <v>1</v>
@@ -6173,7 +6060,7 @@
         <v>2.9110802754338714</v>
       </c>
       <c r="U105" s="26" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="V105" s="26">
         <v>17</v>
@@ -6181,8 +6068,8 @@
       <c r="W105" s="24">
         <v>36.08</v>
       </c>
-      <c r="X105" s="26" t="s">
-        <v>221</v>
+      <c r="X105" s="56" t="s">
+        <v>242</v>
       </c>
       <c r="Y105" s="26">
         <v>16</v>
@@ -6191,7 +6078,7 @@
         <v>8.4441500000000005</v>
       </c>
       <c r="AA105" s="26" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AB105" s="26">
         <v>22</v>
@@ -6199,8 +6086,8 @@
       <c r="AC105" s="54">
         <v>1.7932400000000001E-2</v>
       </c>
-      <c r="AD105" s="26" t="s">
-        <v>221</v>
+      <c r="AD105" s="56" t="s">
+        <v>242</v>
       </c>
       <c r="AE105" s="26">
         <v>16</v>
@@ -6209,7 +6096,7 @@
         <v>6.8356199999999997E-3</v>
       </c>
       <c r="AG105" s="26" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AH105" s="26">
         <v>22</v>
@@ -6218,7 +6105,7 @@
         <v>100</v>
       </c>
       <c r="AJ105" s="56" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="AK105" s="26">
         <v>20</v>
@@ -6227,7 +6114,7 @@
         <v>45.528399999999998</v>
       </c>
       <c r="AM105" s="56" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AN105" s="29">
         <v>15</v>
@@ -6235,7 +6122,7 @@
     </row>
     <row r="106" spans="1:40" ht="15.75">
       <c r="A106" s="11" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B106" s="22">
         <v>5409.9868298857464</v>
@@ -6272,13 +6159,13 @@
         <v>1.5234299999999999E-2</v>
       </c>
       <c r="P106" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Q106" s="57">
         <v>4.0060722426657005</v>
       </c>
       <c r="R106" s="26" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="S106" s="26">
         <v>1</v>
@@ -6287,7 +6174,7 @@
         <v>2.5012657327109995</v>
       </c>
       <c r="U106" s="26" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="V106" s="26">
         <v>12</v>
@@ -6296,7 +6183,7 @@
         <v>26.116</v>
       </c>
       <c r="X106" s="26" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="Y106" s="26">
         <v>15</v>
@@ -6305,7 +6192,7 @@
         <v>8.4215</v>
       </c>
       <c r="AA106" s="26" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AB106" s="26">
         <v>22</v>
@@ -6314,7 +6201,7 @@
         <v>6.9891500000000004E-3</v>
       </c>
       <c r="AD106" s="26" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="AE106" s="26">
         <v>1</v>
@@ -6323,7 +6210,7 @@
         <v>6.2079700000000002E-3</v>
       </c>
       <c r="AG106" s="56" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="AH106" s="26">
         <v>1</v>
@@ -6332,7 +6219,7 @@
         <v>91.044499999999999</v>
       </c>
       <c r="AJ106" s="56" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AK106" s="26">
         <v>22</v>
@@ -6341,7 +6228,7 @@
         <v>29.593399999999999</v>
       </c>
       <c r="AM106" s="56" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="AN106" s="29">
         <v>15</v>
@@ -6349,7 +6236,7 @@
     </row>
     <row r="107" spans="1:40" ht="15.75">
       <c r="A107" s="11" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B107" s="22">
         <v>5260.0345031678471</v>
@@ -6386,13 +6273,13 @@
         <v>1.51339E-2</v>
       </c>
       <c r="P107" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q107" s="57">
         <v>3.4559785684339444</v>
       </c>
       <c r="R107" s="26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="S107" s="26">
         <v>15</v>
@@ -6401,7 +6288,7 @@
         <v>2.2530468183317844</v>
       </c>
       <c r="U107" s="26" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="V107" s="26">
         <v>12</v>
@@ -6410,7 +6297,7 @@
         <v>16.1465</v>
       </c>
       <c r="X107" s="26" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="Y107" s="26">
         <v>16</v>
@@ -6419,7 +6306,7 @@
         <v>8.2277799999999992</v>
       </c>
       <c r="AA107" s="26" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AB107" s="26">
         <v>22</v>
@@ -6428,7 +6315,7 @@
         <v>6.0840499999999997E-3</v>
       </c>
       <c r="AD107" s="26" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="AE107" s="26">
         <v>1</v>
@@ -6437,7 +6324,7 @@
         <v>4.1096300000000004E-3</v>
       </c>
       <c r="AG107" s="56" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AH107" s="26">
         <v>3</v>
@@ -6446,7 +6333,7 @@
         <v>61.274999999999999</v>
       </c>
       <c r="AJ107" s="56" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AK107" s="26">
         <v>22</v>
@@ -6455,7 +6342,7 @@
         <v>36.474899999999998</v>
       </c>
       <c r="AM107" s="56" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AN107" s="29">
         <v>16</v>
@@ -6463,7 +6350,7 @@
     </row>
     <row r="108" spans="1:40" ht="15.75">
       <c r="A108" s="11" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B108" s="22">
         <v>4880.3428688729146</v>
@@ -6500,13 +6387,13 @@
         <v>1.5748100000000001E-2</v>
       </c>
       <c r="P108" s="12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q108" s="59">
         <v>4.2504539844715268</v>
       </c>
       <c r="R108" s="60" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="S108" s="61">
         <v>10</v>
@@ -6515,7 +6402,7 @@
         <v>2.7325462089602159</v>
       </c>
       <c r="U108" s="60" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="V108" s="61">
         <v>17</v>
@@ -6533,7 +6420,7 @@
         <v>8.4485600000000005</v>
       </c>
       <c r="AA108" s="60" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AB108" s="61">
         <v>22</v>
@@ -6542,7 +6429,7 @@
         <v>6.9891500000000004E-3</v>
       </c>
       <c r="AD108" s="60" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="AE108" s="61">
         <v>1</v>
@@ -6551,7 +6438,7 @@
         <v>6.2079700000000002E-3</v>
       </c>
       <c r="AG108" s="63" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="AH108" s="61">
         <v>1</v>
@@ -6560,7 +6447,7 @@
         <v>90.877200000000002</v>
       </c>
       <c r="AJ108" s="63" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="AK108" s="61">
         <v>22</v>
@@ -6577,7 +6464,7 @@
     </row>
     <row r="109" spans="1:40" ht="15.75">
       <c r="A109" s="11" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B109" s="22">
         <v>3938.7143150582915</v>
@@ -6614,12 +6501,12 @@
         <v>1.68863E-2</v>
       </c>
       <c r="P109" s="7" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="110" spans="1:40" ht="15.75">
       <c r="A110" s="11" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B110" s="22">
         <v>3923.956305130047</v>
@@ -6658,7 +6545,7 @@
     </row>
     <row r="111" spans="1:40" ht="15.75">
       <c r="A111" s="11" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B111" s="22">
         <v>4122.5715830260397</v>
@@ -6697,7 +6584,7 @@
     </row>
     <row r="112" spans="1:40" ht="15.75">
       <c r="A112" s="12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B112" s="40">
         <v>3877.3844587743106</v>
@@ -6737,7 +6624,7 @@
     <row r="115" spans="1:12">
       <c r="A115" s="6"/>
       <c r="B115" s="6" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
@@ -6766,14 +6653,14 @@
     </row>
     <row r="117" spans="1:12">
       <c r="A117" s="11"/>
-      <c r="B117" s="70" t="s">
-        <v>152</v>
-      </c>
-      <c r="C117" s="71"/>
-      <c r="D117" s="71"/>
-      <c r="E117" s="72"/>
+      <c r="B117" s="74" t="s">
+        <v>149</v>
+      </c>
+      <c r="C117" s="75"/>
+      <c r="D117" s="75"/>
+      <c r="E117" s="76"/>
       <c r="F117" s="11" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="I117" s="18" t="s">
         <v>71</v>
@@ -6784,7 +6671,7 @@
     </row>
     <row r="118" spans="1:12">
       <c r="A118" s="11" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B118" s="18" t="s">
         <v>81</v>
@@ -6808,43 +6695,43 @@
         <v>86</v>
       </c>
       <c r="I118" s="18" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="J118" s="47" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K118" s="18" t="s">
         <v>90</v>
       </c>
       <c r="L118" s="15" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="119" spans="1:12">
       <c r="A119" s="12"/>
       <c r="B119" s="19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C119" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D119" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E119" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F119" s="19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G119" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H119" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I119" s="19" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J119" s="48"/>
       <c r="K119" s="19" t="s">
@@ -6855,8 +6742,8 @@
       </c>
     </row>
     <row r="120" spans="1:12" ht="15.75">
-      <c r="A120" s="73" t="s">
-        <v>240</v>
+      <c r="A120" s="70" t="s">
+        <v>235</v>
       </c>
       <c r="B120" s="22">
         <f>C120+D120+E120</f>
@@ -6887,7 +6774,7 @@
       <c r="J120" s="50">
         <v>3.8447963185478624</v>
       </c>
-      <c r="K120" s="74">
+      <c r="K120" s="71">
         <v>16.791666666666664</v>
       </c>
       <c r="L120" s="55">
@@ -6895,8 +6782,8 @@
       </c>
     </row>
     <row r="121" spans="1:12" ht="15.75">
-      <c r="A121" s="75" t="s">
-        <v>241</v>
+      <c r="A121" s="72" t="s">
+        <v>236</v>
       </c>
       <c r="B121" s="40">
         <f>C121+D121+E121</f>
@@ -6921,7 +6808,7 @@
       <c r="H121" s="43">
         <v>3810.36375</v>
       </c>
-      <c r="I121" s="76">
+      <c r="I121" s="73">
         <v>1.1168362500000001E-2</v>
       </c>
       <c r="J121" s="65">
@@ -6937,7 +6824,7 @@
     <row r="124" spans="1:12">
       <c r="A124" s="6"/>
       <c r="B124" s="6" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
@@ -6966,14 +6853,14 @@
     </row>
     <row r="126" spans="1:12">
       <c r="A126" s="11"/>
-      <c r="B126" s="70" t="s">
-        <v>152</v>
-      </c>
-      <c r="C126" s="71"/>
-      <c r="D126" s="71"/>
-      <c r="E126" s="72"/>
+      <c r="B126" s="74" t="s">
+        <v>149</v>
+      </c>
+      <c r="C126" s="75"/>
+      <c r="D126" s="75"/>
+      <c r="E126" s="76"/>
       <c r="F126" s="11" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="I126" s="18" t="s">
         <v>71</v>
@@ -6984,7 +6871,7 @@
     </row>
     <row r="127" spans="1:12">
       <c r="A127" s="11" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B127" s="18" t="s">
         <v>81</v>
@@ -7008,43 +6895,43 @@
         <v>86</v>
       </c>
       <c r="I127" s="18" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="J127" s="47" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K127" s="18" t="s">
         <v>90</v>
       </c>
       <c r="L127" s="15" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="128" spans="1:12">
       <c r="A128" s="12"/>
       <c r="B128" s="19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C128" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D128" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E128" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F128" s="19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G128" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H128" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I128" s="19" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J128" s="48"/>
       <c r="K128" s="19" t="s">
@@ -7055,8 +6942,8 @@
       </c>
     </row>
     <row r="129" spans="1:12" ht="15.75">
-      <c r="A129" s="73" t="s">
-        <v>240</v>
+      <c r="A129" s="70" t="s">
+        <v>235</v>
       </c>
       <c r="B129" s="22">
         <f>C129+D129+E129</f>
@@ -7087,7 +6974,7 @@
       <c r="J129" s="50">
         <v>3.543099854148672</v>
       </c>
-      <c r="K129" s="74">
+      <c r="K129" s="71">
         <v>16.791666666666664</v>
       </c>
       <c r="L129" s="55">
@@ -7095,8 +6982,8 @@
       </c>
     </row>
     <row r="130" spans="1:12" ht="15.75">
-      <c r="A130" s="75" t="s">
-        <v>241</v>
+      <c r="A130" s="72" t="s">
+        <v>236</v>
       </c>
       <c r="B130" s="40">
         <f>C130+D130+E130</f>
@@ -7121,7 +7008,7 @@
       <c r="H130" s="43">
         <v>7.2904616666666638E-13</v>
       </c>
-      <c r="I130" s="76">
+      <c r="I130" s="73">
         <v>6.2079700000000036E-3</v>
       </c>
       <c r="J130" s="65">

</xml_diff>